<commit_message>
added the last experiment
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Dataset</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>1,2182,1365932,93620598</t>
+  </si>
+  <si>
+    <t>1,781,37525,1762703</t>
   </si>
 </sst>
 </file>
@@ -286,9 +289,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -343,6 +343,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,6 +668,9 @@
                 <c:pt idx="2">
                   <c:v>135123.28219413699</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>795097.58329391398</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -680,11 +686,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1150582464"/>
-        <c:axId val="1150583008"/>
+        <c:axId val="-1046808832"/>
+        <c:axId val="-1046807200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1150582464"/>
+        <c:axId val="-1046808832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,7 +789,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150583008"/>
+        <c:crossAx val="-1046807200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -791,7 +797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1150583008"/>
+        <c:axId val="-1046807200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1150582464"/>
+        <c:crossAx val="-1046808832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1169,13 +1175,15 @@
                 <c:pt idx="2">
                   <c:v>6840572</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>1823430493</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1184,11 +1192,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1154252672"/>
-        <c:axId val="1154258112"/>
+        <c:axId val="-1046814816"/>
+        <c:axId val="-1046811552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1154252672"/>
+        <c:axId val="-1046814816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,13 +1223,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>File DB</a:t>
+                  <a:t>File DB size</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> size</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1256,7 +1259,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1292,7 +1295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1154258112"/>
+        <c:crossAx val="-1046811552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1300,7 +1303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1154258112"/>
+        <c:axId val="-1046811552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1377,7 +1380,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1407,7 +1410,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1154252672"/>
+        <c:crossAx val="-1046814816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2614,15 +2617,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:colOff>1724025</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2934,7 +2937,7 @@
   <dimension ref="C2:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2955,24 +2958,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="35" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="35"/>
-      <c r="M2" s="36"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="35"/>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2996,53 +2999,53 @@
       <c r="J3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <v>108</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="18">
         <v>1000</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="18">
         <v>563</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="18">
         <v>50</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="19">
         <v>6.0193538665771396</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="20">
         <v>13455</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="26" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -3072,15 +3075,15 @@
       <c r="L5" s="12">
         <v>2889</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -3107,12 +3110,12 @@
       <c r="L6" s="8">
         <v>1133131</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="28" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>4</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -3142,15 +3145,15 @@
       <c r="L7" s="12">
         <v>33346</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="30">
+      <c r="C8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -3177,12 +3180,12 @@
       <c r="L8" s="8">
         <v>254969682</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>6</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -3212,15 +3215,15 @@
       <c r="L9" s="12">
         <v>6840572</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="30">
+      <c r="C10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="30" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -3247,12 +3250,12 @@
       <c r="L10" s="8">
         <v>98567529593</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="28" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>8</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -3270,13 +3273,21 @@
       <c r="H11" s="13">
         <v>75000</v>
       </c>
-      <c r="I11" s="13"/>
+      <c r="I11" s="13">
+        <v>21946</v>
+      </c>
       <c r="J11" s="13">
         <v>50</v>
       </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="K11" s="15">
+        <v>795097.58329391398</v>
+      </c>
+      <c r="L11" s="16">
+        <v>1823430493</v>
+      </c>
+      <c r="M11" s="36" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">

</xml_diff>

<commit_message>
add new algorithm ImprovedBasic
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -10,15 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$I$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$I$33</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
   <si>
     <t>Dataset</t>
   </si>
@@ -104,9 +103,6 @@
     <t>1, 20, 33, 33</t>
   </si>
   <si>
-    <t>http://statistical-research.com/association-rule-learning-and-the-apriori-algorithm/</t>
-  </si>
-  <si>
     <t>dataset-88162.csv</t>
   </si>
   <si>
@@ -114,9 +110,6 @@
   </si>
   <si>
     <t>50, 200, 1000, 10000</t>
-  </si>
-  <si>
-    <t>New approach</t>
   </si>
   <si>
     <t>1, 13, 80, 81</t>
@@ -132,6 +125,27 @@
   </si>
   <si>
     <t>1, 23, 100, 1384</t>
+  </si>
+  <si>
+    <t>ImprovedBasic</t>
+  </si>
+  <si>
+    <t>ImprovedOptimized</t>
+  </si>
+  <si>
+    <t>1, 68, 300, 432</t>
+  </si>
+  <si>
+    <t>1, 261, 9763, 26168</t>
+  </si>
+  <si>
+    <t>1, 786, 46073, 2250887</t>
+  </si>
+  <si>
+    <t>1, 2182, 1351490, 92628214</t>
+  </si>
+  <si>
+    <t>1, 3392, 1403166, 32272345</t>
   </si>
 </sst>
 </file>
@@ -158,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,8 +209,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -287,7 +307,50 @@
         <color theme="0" tint="-0.499984740745262"/>
       </top>
       <bottom style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -298,7 +361,7 @@
         <color theme="0" tint="-0.499984740745262"/>
       </top>
       <bottom style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -311,7 +374,7 @@
         <color theme="0" tint="-0.499984740745262"/>
       </top>
       <bottom style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -319,14 +382,12 @@
       <left style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
+      <right/>
       <top style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -334,10 +395,10 @@
       <left/>
       <right/>
       <top style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -347,10 +408,10 @@
         <color theme="0" tint="-0.499984740745262"/>
       </right>
       <top style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -358,11 +419,9 @@
       <left style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
+      <right/>
       <top style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.499984740745262"/>
@@ -373,7 +432,7 @@
       <left/>
       <right/>
       <top style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.499984740745262"/>
@@ -386,7 +445,7 @@
         <color theme="0" tint="-0.499984740745262"/>
       </right>
       <top style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.499984740745262"/>
@@ -397,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -414,94 +473,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,6 +487,120 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,7 +771,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$H$9,Sheet1!$H$13,Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -710,7 +795,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$K$6,Sheet1!$K$10,Sheet1!$K$14,Sheet1!$K$18,Sheet1!$K$22)</c:f>
+              <c:f>(Sheet1!$K$6,Sheet1!$K$11,Sheet1!$K$16,Sheet1!$K$21,Sheet1!$K$26)</c:f>
               <c:numCache>
                 <c:formatCode>0.00000000000000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -728,6 +813,130 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>85.112333297729407</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ImprovedBasic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88162</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$K$7,Sheet1!$K$12,Sheet1!$K$17,Sheet1!$K$22,Sheet1!$K$27)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000000000000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19.5257663726806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>399.88565444946198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4509.5803737640299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57903.233051299998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3538.6459827423</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -736,7 +945,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Optimized algorithm</c:v>
           </c:tx>
@@ -810,7 +1019,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$H$9,Sheet1!$H$13,Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -834,7 +1043,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$K$7,Sheet1!$K$11,Sheet1!$K$15,Sheet1!$K$19,Sheet1!$K$23)</c:f>
+              <c:f>(Sheet1!$K$8,Sheet1!$K$13,Sheet1!$K$18,Sheet1!$K$23,Sheet1!$K$28)</c:f>
               <c:numCache>
                 <c:formatCode>0.00000000000000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -852,6 +1061,130 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>30892.0001983642</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>ImprovedOptimized</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88162</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$K$9,Sheet1!$K$14,Sheet1!$K$19,Sheet1!$K$24,Sheet1!$K$29)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000000000000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1299.00670051574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20098.488330840999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>315073.44937324501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1766863.0604743899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26854.609012603702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,7 +1193,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>Hypergraph</c:v>
           </c:tx>
@@ -934,7 +1267,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$H$9,Sheet1!$H$13,Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -958,7 +1291,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$K$8,Sheet1!$K$12,Sheet1!$K$16,Sheet1!$K$20,Sheet1!$K$24)</c:f>
+              <c:f>(Sheet1!$K$10,Sheet1!$K$15,Sheet1!$K$20,Sheet1!$K$25,Sheet1!$K$30)</c:f>
               <c:numCache>
                 <c:formatCode>0.00000000000000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -967,130 +1300,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2138392.0021057101</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>New approach</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="35000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="51000"/>
-                      <a:satMod val="130000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="80000">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="93000"/>
-                      <a:satMod val="130000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="94000"/>
-                      <a:satMod val="135000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="16200000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="35000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:scene3d>
-                <a:camera prst="orthographicFront">
-                  <a:rot lat="0" lon="0" rev="0"/>
-                </a:camera>
-                <a:lightRig rig="threePt" dir="t">
-                  <a:rot lat="0" lon="0" rev="1200000"/>
-                </a:lightRig>
-              </a:scene3d>
-              <a:sp3d>
-                <a:bevelT w="63500" h="25400"/>
-              </a:sp3d>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>(Sheet1!$H$9,Sheet1!$H$13,Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>88162</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(Sheet1!$K$9,Sheet1!$K$13,Sheet1!$K$17,Sheet1!$K$21,Sheet1!$K$25)</c:f>
-              <c:numCache>
-                <c:formatCode>0.00000000000000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1299.00670051574</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20098.488330840999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>315073.44937324501</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1766863.0604743899</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>26854.609012603702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1107,11 +1316,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1854836176"/>
-        <c:axId val="-1854831824"/>
+        <c:axId val="243102208"/>
+        <c:axId val="243103296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1854836176"/>
+        <c:axId val="243102208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +1419,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1854831824"/>
+        <c:crossAx val="243103296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1218,7 +1427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1854831824"/>
+        <c:axId val="243103296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1854836176"/>
+        <c:crossAx val="243102208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1564,7 +1773,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$H$9,Sheet1!$H$13,Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1588,7 +1797,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$L$6,Sheet1!$L$10,Sheet1!$L$14,Sheet1!$L$18,Sheet1!$L$22)</c:f>
+              <c:f>(Sheet1!$L$6,Sheet1!$L$11,Sheet1!$L$16,Sheet1!$L$21,Sheet1!$L$26)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1606,6 +1815,130 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>217179912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ImprovedBasic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88162</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$L$7,Sheet1!$L$12,Sheet1!$L$17,Sheet1!$L$22,Sheet1!$L$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10489</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1031133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>249044449</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97522501305</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>216999168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1614,7 +1947,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Optimized algorithm</c:v>
           </c:tx>
@@ -1688,7 +2021,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$H$9,Sheet1!$H$13,Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1712,7 +2045,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$L$7,Sheet1!$L$11,Sheet1!$L$15,Sheet1!$L$19,Sheet1!$L$23)</c:f>
+              <c:f>(Sheet1!$L$8,Sheet1!$L$13,Sheet1!$L$18,Sheet1!$L$23,Sheet1!$L$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1730,6 +2063,130 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>30610</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>ImprovedOptimized</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88162</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$L$9,Sheet1!$L$14,Sheet1!$L$18,Sheet1!$L$24,Sheet1!$L$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2525</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25904</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1738,7 +2195,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>Hypergraph</c:v>
           </c:tx>
@@ -1812,7 +2269,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$H$9,Sheet1!$H$13,Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
+              <c:f>(Sheet1!$H$7,Sheet1!$H$12,Sheet1!$H$17,Sheet1!$H$22,Sheet1!$H$27)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1836,7 +2293,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$L$8,Sheet1!$L$12,Sheet1!$L$16,Sheet1!$L$20,Sheet1!$L$24)</c:f>
+              <c:f>(Sheet1!$L$10,Sheet1!$L$15,Sheet1!$L$20,Sheet1!$L$25,Sheet1!$L$30)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1845,130 +2302,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2536</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>New approach</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="35000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="51000"/>
-                      <a:satMod val="130000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="80000">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="93000"/>
-                      <a:satMod val="130000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:shade val="94000"/>
-                      <a:satMod val="135000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="16200000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="35000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:scene3d>
-                <a:camera prst="orthographicFront">
-                  <a:rot lat="0" lon="0" rev="0"/>
-                </a:camera>
-                <a:lightRig rig="threePt" dir="t">
-                  <a:rot lat="0" lon="0" rev="1200000"/>
-                </a:lightRig>
-              </a:scene3d>
-              <a:sp3d>
-                <a:bevelT w="63500" h="25400"/>
-              </a:sp3d>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>(Sheet1!$H$9,Sheet1!$H$13,Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>88162</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(Sheet1!$L$9,Sheet1!$L$13,Sheet1!$L$17,Sheet1!$L$21,Sheet1!$L$25)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1360</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2525</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8266</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25904</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1985,11 +2318,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1854839440"/>
-        <c:axId val="-1854829648"/>
+        <c:axId val="287189424"/>
+        <c:axId val="287182352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1854839440"/>
+        <c:axId val="287189424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,7 +2421,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1854829648"/>
+        <c:crossAx val="287182352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2096,7 +2429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1854829648"/>
+        <c:axId val="287182352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2203,7 +2536,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1854839440"/>
+        <c:crossAx val="287189424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3380,13 +3713,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3409,14 +3742,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1152525</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>914401</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3726,27 +4059,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M79"/>
+  <dimension ref="C2:M41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.375" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.375" customWidth="1"/>
+    <col min="7" max="7" width="19.125" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="9" width="14.75" customWidth="1"/>
+    <col min="10" max="10" width="12.125" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.125" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.875" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
@@ -3757,21 +4090,21 @@
       </c>
     </row>
     <row r="4" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="42" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="43"/>
-      <c r="M4" s="44"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
@@ -3793,7 +4126,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>3</v>
@@ -3809,37 +4142,37 @@
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="8">
+      <c r="C6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="25">
         <v>108</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="25">
         <v>1000</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="25">
         <v>563</v>
       </c>
-      <c r="J6" s="36">
+      <c r="J6" s="27">
         <v>50</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="28">
         <v>6.0193538665771396</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="29">
         <v>13455</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="30" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3847,69 +4180,69 @@
       <c r="C7" s="14">
         <v>2</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="16" t="s">
+      <c r="D7" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="33">
         <v>108</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="33">
         <v>1000</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="33">
         <v>563</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="35">
         <v>50</v>
       </c>
-      <c r="K7" s="28">
-        <v>1331.16149902343</v>
-      </c>
-      <c r="L7" s="18">
-        <v>1700</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>20</v>
+      <c r="K7" s="36">
+        <v>19.5257663726806</v>
+      </c>
+      <c r="L7" s="37">
+        <v>10489</v>
+      </c>
+      <c r="M7" s="38" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C8" s="14">
         <v>3</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="33">
         <v>108</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="33">
         <v>1000</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="33">
         <v>563</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="35">
         <v>50</v>
       </c>
-      <c r="K8" s="28">
-        <v>123820.62649726799</v>
-      </c>
-      <c r="L8" s="18">
+      <c r="K8" s="36">
+        <v>1331.16149902343</v>
+      </c>
+      <c r="L8" s="37">
         <v>1700</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="38" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3917,595 +4250,777 @@
       <c r="C9" s="14">
         <v>4</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="D9" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="33">
         <v>108</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="33">
         <v>1000</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="33">
         <v>563</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="35">
         <v>50</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="36">
         <v>1299.00670051574</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="37">
         <v>1360</v>
       </c>
-      <c r="M9" s="19" t="s">
-        <v>33</v>
+      <c r="M9" s="38" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="20">
+      <c r="C10" s="14">
         <v>5</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="21">
-        <v>554</v>
-      </c>
-      <c r="G10" s="23" t="s">
+      <c r="D10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="33">
+        <v>108</v>
+      </c>
+      <c r="G10" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="21">
-        <v>5000</v>
-      </c>
-      <c r="I10" s="21">
-        <v>2339</v>
-      </c>
-      <c r="J10" s="37">
+      <c r="H10" s="33">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="33">
+        <v>563</v>
+      </c>
+      <c r="J10" s="35">
         <v>50</v>
       </c>
-      <c r="K10" s="26">
-        <v>24.721145629882798</v>
-      </c>
-      <c r="L10" s="24">
-        <v>1133131</v>
-      </c>
-      <c r="M10" s="25" t="s">
-        <v>22</v>
+      <c r="K10" s="36">
+        <v>123820.62649726799</v>
+      </c>
+      <c r="L10" s="37">
+        <v>1700</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="20">
+      <c r="C11" s="15">
         <v>6</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="22" t="s">
+      <c r="D11" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="41">
         <v>554</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="41">
         <v>5000</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="41">
         <v>2339</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="43">
         <v>50</v>
       </c>
-      <c r="K11" s="26">
-        <v>21073.792457580501</v>
-      </c>
-      <c r="L11" s="24">
-        <v>2536</v>
-      </c>
-      <c r="M11" s="25" t="s">
-        <v>27</v>
+      <c r="K11" s="44">
+        <v>24.721145629882798</v>
+      </c>
+      <c r="L11" s="45">
+        <v>1133131</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="20">
+      <c r="C12" s="15">
         <v>7</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="22" t="s">
+      <c r="D12" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="41">
         <v>554</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="41">
         <v>5000</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="41">
         <v>2339</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="43">
         <v>50</v>
       </c>
-      <c r="K12" s="26">
-        <v>2138392.0021057101</v>
-      </c>
-      <c r="L12" s="24">
-        <v>2536</v>
-      </c>
-      <c r="M12" s="25" t="s">
-        <v>27</v>
+      <c r="K12" s="44">
+        <v>399.88565444946198</v>
+      </c>
+      <c r="L12" s="45">
+        <v>1031133</v>
+      </c>
+      <c r="M12" s="46" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="20">
+      <c r="C13" s="15">
         <v>8</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="22" t="s">
+      <c r="D13" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="41">
         <v>554</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="41">
         <v>5000</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="41">
         <v>2339</v>
       </c>
-      <c r="J13" s="37">
+      <c r="J13" s="43">
         <v>50</v>
       </c>
-      <c r="K13" s="26">
-        <v>20098.488330840999</v>
-      </c>
-      <c r="L13" s="24">
-        <v>2525</v>
-      </c>
-      <c r="M13" s="25" t="s">
-        <v>34</v>
+      <c r="K13" s="44">
+        <v>21073.792457580501</v>
+      </c>
+      <c r="L13" s="45">
+        <v>2536</v>
+      </c>
+      <c r="M13" s="46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="14">
+      <c r="C14" s="15">
         <v>9</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="15">
-        <v>2197</v>
-      </c>
-      <c r="G14" s="17" t="s">
+      <c r="D14" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="41">
+        <v>554</v>
+      </c>
+      <c r="G14" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="15">
-        <v>20000</v>
-      </c>
-      <c r="I14" s="15">
-        <v>7199</v>
-      </c>
-      <c r="J14" s="27">
+      <c r="H14" s="41">
+        <v>5000</v>
+      </c>
+      <c r="I14" s="41">
+        <v>2339</v>
+      </c>
+      <c r="J14" s="43">
         <v>50</v>
       </c>
-      <c r="K14" s="28">
-        <v>77.183961868286104</v>
-      </c>
-      <c r="L14" s="18">
-        <v>254969682</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>23</v>
+      <c r="K14" s="44">
+        <v>20098.488330840999</v>
+      </c>
+      <c r="L14" s="45">
+        <v>2525</v>
+      </c>
+      <c r="M14" s="46" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="14">
+      <c r="C15" s="15">
         <v>10</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="15">
-        <v>2197</v>
-      </c>
-      <c r="G15" s="17" t="s">
+      <c r="D15" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="41">
+        <v>554</v>
+      </c>
+      <c r="G15" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="15">
-        <v>20000</v>
-      </c>
-      <c r="I15" s="15">
-        <v>7199</v>
-      </c>
-      <c r="J15" s="27">
+      <c r="H15" s="41">
+        <v>5000</v>
+      </c>
+      <c r="I15" s="41">
+        <v>2339</v>
+      </c>
+      <c r="J15" s="43">
         <v>50</v>
       </c>
-      <c r="K15" s="28">
-        <v>362305.08613586402</v>
-      </c>
-      <c r="L15" s="18">
-        <v>8266</v>
-      </c>
-      <c r="M15" s="19" t="s">
-        <v>24</v>
+      <c r="K15" s="44">
+        <v>2138392.0021057101</v>
+      </c>
+      <c r="L15" s="45">
+        <v>2536</v>
+      </c>
+      <c r="M15" s="46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C16" s="14">
         <v>11</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="16" t="s">
+      <c r="D16" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="33">
         <v>2197</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="33">
         <v>20000</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="33">
         <v>7199</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16" s="35">
         <v>50</v>
       </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="19"/>
+      <c r="K16" s="36">
+        <v>77.183961868286104</v>
+      </c>
+      <c r="L16" s="37">
+        <v>254969682</v>
+      </c>
+      <c r="M16" s="38" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" s="14">
         <v>12</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="16" t="s">
+      <c r="D17" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="33">
         <v>2197</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="33">
         <v>20000</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="33">
         <v>7199</v>
       </c>
-      <c r="J17" s="27">
+      <c r="J17" s="35">
         <v>50</v>
       </c>
-      <c r="K17" s="28">
-        <v>315073.44937324501</v>
-      </c>
-      <c r="L17" s="18">
-        <v>8266</v>
-      </c>
-      <c r="M17" s="19" t="s">
-        <v>24</v>
+      <c r="K17" s="36">
+        <v>4509.5803737640299</v>
+      </c>
+      <c r="L17" s="37">
+        <v>249044449</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="20">
+      <c r="C18" s="14">
         <v>13</v>
       </c>
-      <c r="D18" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="21">
-        <v>8193</v>
-      </c>
-      <c r="G18" s="23" t="s">
+      <c r="D18" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="33">
+        <v>2197</v>
+      </c>
+      <c r="G18" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="21">
-        <v>75000</v>
-      </c>
-      <c r="I18" s="21">
-        <v>21946</v>
-      </c>
-      <c r="J18" s="37">
+      <c r="H18" s="33">
+        <v>20000</v>
+      </c>
+      <c r="I18" s="33">
+        <v>7199</v>
+      </c>
+      <c r="J18" s="35">
         <v>50</v>
       </c>
-      <c r="K18" s="26">
-        <v>236.849069595336</v>
-      </c>
-      <c r="L18" s="24">
-        <v>98567529593</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>25</v>
+      <c r="K18" s="36">
+        <v>362305.08613586402</v>
+      </c>
+      <c r="L18" s="37">
+        <v>8266</v>
+      </c>
+      <c r="M18" s="38" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C19" s="20">
+      <c r="C19" s="14">
         <v>14</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="21">
-        <v>8193</v>
-      </c>
-      <c r="G19" s="23" t="s">
+      <c r="D19" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="33">
+        <v>2197</v>
+      </c>
+      <c r="G19" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="21">
-        <v>75000</v>
-      </c>
-      <c r="I19" s="21">
-        <v>21946</v>
-      </c>
-      <c r="J19" s="37">
+      <c r="H19" s="33">
+        <v>20000</v>
+      </c>
+      <c r="I19" s="33">
+        <v>7199</v>
+      </c>
+      <c r="J19" s="35">
         <v>50</v>
       </c>
-      <c r="K19" s="26">
-        <v>1777466.3765430399</v>
-      </c>
-      <c r="L19" s="24">
-        <v>25904</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>26</v>
+      <c r="K19" s="36">
+        <v>315073.44937324501</v>
+      </c>
+      <c r="L19" s="37">
+        <v>8266</v>
+      </c>
+      <c r="M19" s="38" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C20" s="20">
+      <c r="C20" s="14">
         <v>15</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="21">
-        <v>8193</v>
-      </c>
-      <c r="G20" s="23" t="s">
+      <c r="E20" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="33">
+        <v>2197</v>
+      </c>
+      <c r="G20" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="21">
-        <v>75000</v>
-      </c>
-      <c r="I20" s="21">
-        <v>21946</v>
-      </c>
-      <c r="J20" s="37">
+      <c r="H20" s="33">
+        <v>20000</v>
+      </c>
+      <c r="I20" s="33">
+        <v>7199</v>
+      </c>
+      <c r="J20" s="35">
         <v>50</v>
       </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="38"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C21" s="20">
+      <c r="C21" s="15">
         <v>16</v>
       </c>
-      <c r="D21" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="22" t="s">
+      <c r="D21" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="41">
         <v>8193</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="41">
         <v>75000</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="41">
         <v>21946</v>
       </c>
-      <c r="J21" s="37">
+      <c r="J21" s="43">
         <v>50</v>
       </c>
-      <c r="K21" s="26">
-        <v>1766863.0604743899</v>
-      </c>
-      <c r="L21" s="24">
-        <v>25904</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>26</v>
+      <c r="K21" s="44">
+        <v>236.849069595336</v>
+      </c>
+      <c r="L21" s="45">
+        <v>98567529593</v>
+      </c>
+      <c r="M21" s="46" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="14">
+      <c r="C22" s="15">
         <v>17</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="15">
-        <v>50675</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="15">
-        <v>88162</v>
-      </c>
-      <c r="I22" s="15">
-        <v>8273</v>
-      </c>
-      <c r="J22" s="27">
-        <v>16470</v>
-      </c>
-      <c r="K22" s="28">
-        <v>85.112333297729407</v>
-      </c>
-      <c r="L22" s="18">
-        <v>217179912</v>
-      </c>
-      <c r="M22" s="19" t="s">
-        <v>30</v>
+      <c r="D22" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="41">
+        <v>8193</v>
+      </c>
+      <c r="G22" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="41">
+        <v>75000</v>
+      </c>
+      <c r="I22" s="41">
+        <v>21946</v>
+      </c>
+      <c r="J22" s="43">
+        <v>50</v>
+      </c>
+      <c r="K22" s="44">
+        <v>57903.233051299998</v>
+      </c>
+      <c r="L22" s="45">
+        <v>97522501305</v>
+      </c>
+      <c r="M22" s="46" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C23" s="14">
+      <c r="C23" s="15">
         <v>18</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="15">
-        <v>50675</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="15">
-        <v>88162</v>
-      </c>
-      <c r="I23" s="15">
-        <v>8273</v>
-      </c>
-      <c r="J23" s="27">
-        <v>16470</v>
-      </c>
-      <c r="K23" s="28">
-        <v>30892.0001983642</v>
-      </c>
-      <c r="L23" s="18">
-        <v>30610</v>
-      </c>
-      <c r="M23" s="19" t="s">
-        <v>37</v>
+      <c r="E23" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="41">
+        <v>8193</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="41">
+        <v>75000</v>
+      </c>
+      <c r="I23" s="41">
+        <v>21946</v>
+      </c>
+      <c r="J23" s="43">
+        <v>50</v>
+      </c>
+      <c r="K23" s="44">
+        <v>1777466.3765430399</v>
+      </c>
+      <c r="L23" s="45">
+        <v>25904</v>
+      </c>
+      <c r="M23" s="46" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="14">
+      <c r="C24" s="15">
         <v>19</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="15">
-        <v>50675</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="15">
-        <v>88162</v>
-      </c>
-      <c r="I24" s="15">
-        <v>8273</v>
-      </c>
-      <c r="J24" s="27">
-        <v>16470</v>
-      </c>
-      <c r="K24" s="28"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="19"/>
+      <c r="D24" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="41">
+        <v>8193</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="41">
+        <v>75000</v>
+      </c>
+      <c r="I24" s="41">
+        <v>21946</v>
+      </c>
+      <c r="J24" s="43">
+        <v>50</v>
+      </c>
+      <c r="K24" s="44">
+        <v>1766863.0604743899</v>
+      </c>
+      <c r="L24" s="45">
+        <v>25904</v>
+      </c>
+      <c r="M24" s="46" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C25" s="29">
+      <c r="C25" s="15">
         <v>20</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="31" t="s">
+      <c r="D25" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="41">
+        <v>8193</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="41">
+        <v>75000</v>
+      </c>
+      <c r="I25" s="41">
+        <v>21946</v>
+      </c>
+      <c r="J25" s="43">
+        <v>50</v>
+      </c>
+      <c r="K25" s="44"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="46"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C26" s="14">
+        <v>21</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="33">
+        <v>50675</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="33">
+        <v>88162</v>
+      </c>
+      <c r="I26" s="33">
+        <v>8273</v>
+      </c>
+      <c r="J26" s="35">
+        <v>16470</v>
+      </c>
+      <c r="K26" s="36">
+        <v>85.112333297729407</v>
+      </c>
+      <c r="L26" s="37">
+        <v>217179912</v>
+      </c>
+      <c r="M26" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="30">
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C27" s="14">
+        <v>22</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="33">
         <v>50675</v>
       </c>
-      <c r="G25" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="30">
+      <c r="G27" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="33">
         <v>88162</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I27" s="33">
         <v>8273</v>
       </c>
-      <c r="J25" s="38">
+      <c r="J27" s="35">
         <v>16470</v>
       </c>
-      <c r="K25" s="32">
-        <v>26854.609012603702</v>
-      </c>
-      <c r="L25" s="33">
-        <v>24862</v>
-      </c>
-      <c r="M25" s="34" t="s">
-        <v>36</v>
+      <c r="K27" s="36">
+        <v>3538.6459827423</v>
+      </c>
+      <c r="L27" s="37">
+        <v>216999168</v>
+      </c>
+      <c r="M27" s="38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C28" s="14">
+        <v>23</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="33">
+        <v>50675</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="33">
+        <v>88162</v>
+      </c>
+      <c r="I28" s="33">
+        <v>8273</v>
+      </c>
+      <c r="J28" s="35">
+        <v>16470</v>
+      </c>
+      <c r="K28" s="36">
+        <v>30892.0001983642</v>
+      </c>
+      <c r="L28" s="37">
+        <v>30610</v>
+      </c>
+      <c r="M28" s="38" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I29" s="1"/>
+      <c r="C29" s="14">
+        <v>24</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="33">
+        <v>50675</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="33">
+        <v>88162</v>
+      </c>
+      <c r="I29" s="33">
+        <v>8273</v>
+      </c>
+      <c r="J29" s="35">
+        <v>16470</v>
+      </c>
+      <c r="K29" s="36">
+        <v>26854.609012603702</v>
+      </c>
+      <c r="L29" s="37">
+        <v>24862</v>
+      </c>
+      <c r="M29" s="38" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G31" s="1"/>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C30" s="16">
+        <v>25</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="49">
+        <v>50675</v>
+      </c>
+      <c r="G30" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="49">
+        <v>88162</v>
+      </c>
+      <c r="I30" s="49">
+        <v>8273</v>
+      </c>
+      <c r="J30" s="51">
+        <v>16470</v>
+      </c>
+      <c r="K30" s="52"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="54"/>
+    </row>
+    <row r="32" spans="3:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="20"/>
     </row>
     <row r="34" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
     <row r="36" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="2"/>
+      <c r="G36" s="1"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>28</v>
-      </c>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>